<commit_message>
Ingest revised PFPC data sources
Note also that `xlrd` no longer supports reading .xlsx files, so I changed my ingestion script to use `openpyxl` instead.
</commit_message>
<xml_diff>
--- a/food-data/PFPC_data_files/Additional Food Bucks sites.xlsx
+++ b/food-data/PFPC_data_files/Additional Food Bucks sites.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewl\Documents\GitHub\food-access-map-data\food-data\PFPC_data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6A0597-1B0D-4620-AEBD-555E845E2F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additional Food Bucks sites" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -42,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -59,15 +65,6 @@
     <t>zip_code</t>
   </si>
   <si>
-    <t>Shop 'n Save</t>
-  </si>
-  <si>
-    <t>336 8th St</t>
-  </si>
-  <si>
-    <t>New Kensington</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -90,12 +87,18 @@
   </si>
   <si>
     <t>see Fresh Corners, Fresh Access, and Green Grocer sheets for more sites</t>
+  </si>
+  <si>
+    <t>East End Food Co-op</t>
+  </si>
+  <si>
+    <t>7516 Meade St</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -108,8 +111,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -121,8 +124,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -138,17 +141,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -473,22 +485,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="2"/>
-    <col min="2" max="2" width="36.83203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="2"/>
+    <col min="2" max="2" width="36.85546875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,60 +519,60 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3">
+        <v>15207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>15301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
-        <v>15068</v>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15208</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>15207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>15301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>